<commit_message>
move LOINC answer codes from ValueSet SPLASCHFrequencyObservationVS to CodeSystem SPLASCHFrequencyCS and include this CS in the VS. Update ObservationSPLASCH fsh file accordingly.
</commit_message>
<xml_diff>
--- a/output/ValueSet-SPLASCHFrequencyObservationVS.xlsx
+++ b/output/ValueSet-SPLASCHFrequencyObservationVS.xlsx
@@ -8,13 +8,13 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include from Observation Valu" r:id="rId4" sheetId="2"/>
-    <sheet name="Include from LOINC" r:id="rId5" sheetId="3"/>
+    <sheet name="Include from Observation Valu 2" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Property</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-29T14:30:00-04:00</t>
+    <t>2022-05-03T12:45:05-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -115,40 +115,7 @@
     <t>http://hl7.org/fhir/us/pacio-splasch/CodeSystem/SPLASCHTimePercentageCategoryCS</t>
   </si>
   <si>
-    <t>Concept</t>
-  </si>
-  <si>
-    <t>LA6270-8</t>
-  </si>
-  <si>
-    <t>Never</t>
-  </si>
-  <si>
-    <t>LA10066-1</t>
-  </si>
-  <si>
-    <t>Rarely</t>
-  </si>
-  <si>
-    <t>LA10082-8</t>
-  </si>
-  <si>
-    <t>Sometimes</t>
-  </si>
-  <si>
-    <t>LA10044-8</t>
-  </si>
-  <si>
-    <t>Often</t>
-  </si>
-  <si>
-    <t>LA9933-8</t>
-  </si>
-  <si>
-    <t>Always</t>
-  </si>
-  <si>
-    <t>http://loinc.org</t>
+    <t>http://hl7.org/fhir/us/pacio-splasch/CodeSystem/SPLASCHFrequencyCS</t>
   </si>
 </sst>
 </file>
@@ -466,7 +433,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -478,66 +445,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>